<commit_message>
Paul Kamau - Task Sheet
</commit_message>
<xml_diff>
--- a/Prime-rebuild/experts/experts.xlsx
+++ b/Prime-rebuild/experts/experts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
+    <workbookView xWindow="480" yWindow="180" windowWidth="27795" windowHeight="12525"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="344">
   <si>
     <t>Name</t>
   </si>
@@ -1450,10 +1450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F119"/>
+  <dimension ref="B1:F121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="B123" sqref="B123"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="B125" sqref="B125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2094,355 +2094,358 @@
     <row r="43" spans="2:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E43" s="10"/>
     </row>
-    <row r="44" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B44" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E44" s="8" t="s">
-        <v>137</v>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B44" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B46" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D45" s="1" t="s">
+      <c r="C46" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E45" s="8" t="s">
+      <c r="E46" s="8" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B46" s="1" t="s">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B47" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C47" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B47" s="1" t="s">
+    <row r="48" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B48" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C47" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D47" s="1" t="s">
+      <c r="C48" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E47" s="8" t="s">
+      <c r="E48" s="8" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="48" spans="2:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="B48" s="1" t="s">
+    <row r="49" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="B49" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="D49" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E48" s="8" t="s">
+      <c r="E49" s="8" t="s">
         <v>147</v>
-      </c>
-    </row>
-    <row r="49" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B49" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="E49" s="8" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="50" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B50" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>19</v>
+        <v>149</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E50" s="8" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="51" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B51" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>157</v>
+        <v>19</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E51" s="8" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="52" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B53" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D52" s="1" t="s">
+      <c r="C53" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="E52" s="8" t="s">
+      <c r="E53" s="8" t="s">
         <v>161</v>
-      </c>
-    </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B53" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="E53" s="8" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B54" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="55" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B55" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B56" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C56" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="D56" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="E55" s="8" t="s">
+      <c r="E56" s="8" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="56" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B56" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="E56" s="8" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="57" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B57" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E57" s="8" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="58" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B58" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E58" s="8" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B59" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C58" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D58" s="1" t="s">
+      <c r="C59" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="E58" s="8" t="s">
+      <c r="E59" s="8" t="s">
         <v>175</v>
-      </c>
-    </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B59" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E59" s="8" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="60" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B60" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E60" s="8" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B61" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="E60" s="8" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="61" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B61" s="1" t="s">
-        <v>181</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D61" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E61" s="8" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B62" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="62" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B62" s="1" t="s">
+    <row r="63" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B63" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="C62" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D62" s="1" t="s">
+      <c r="C63" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D63" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E62" s="8" t="s">
+      <c r="E63" s="8" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="63" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B63" s="1" t="s">
+    <row r="64" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B64" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C64" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D63" s="1" t="s">
+      <c r="D64" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="E63" s="8" t="s">
+      <c r="E64" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="F63" s="1" t="s">
+      <c r="F64" s="1" t="s">
         <v>188</v>
-      </c>
-    </row>
-    <row r="64" spans="2:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="B64" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="E64" s="8" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="65" spans="2:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B65" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E65" s="8" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="B66" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="C66" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D65" s="1" t="s">
+      <c r="D66" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="E65" s="8" t="s">
+      <c r="E66" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="F65" s="2" t="s">
+      <c r="F66" s="2" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B66" s="1" t="s">
+    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B67" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="C66" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D66" s="1" t="s">
+      <c r="C67" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D67" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="E66" s="8" t="s">
+      <c r="E67" s="8" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="67" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B67" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="E67" s="8" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="68" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B68" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>19</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="E68" s="8" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="69" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B69" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B70" s="1" t="s">
         <v>202</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E69" s="8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="70" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B70" s="1" t="s">
-        <v>203</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>10</v>
@@ -2451,719 +2454,750 @@
         <v>82</v>
       </c>
       <c r="E70" s="8" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="71" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B71" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>205</v>
+        <v>82</v>
       </c>
       <c r="E71" s="8" t="s">
-        <v>206</v>
+        <v>139</v>
       </c>
     </row>
     <row r="72" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B72" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E72" s="8" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B73" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D73" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E73" s="8" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B74" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D74" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="E73" s="8" t="s">
+      <c r="E74" s="8" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="74" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B74" s="1" t="s">
+    <row r="75" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B75" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="C74" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D74" s="1" t="s">
+      <c r="C75" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D75" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="E74" s="8" t="s">
+      <c r="E75" s="8" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="75" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B75" s="1" t="s">
+    <row r="76" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B76" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="C75" s="1" t="s">
+      <c r="C76" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D75" s="1" t="s">
+      <c r="D76" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E75" s="8" t="s">
+      <c r="E76" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="F75" s="2" t="s">
+      <c r="F76" s="2" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="76" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B76" s="1" t="s">
+    <row r="77" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B77" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="C76" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D76" s="1" t="s">
+      <c r="C77" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D77" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="E76" s="8" t="s">
+      <c r="E77" s="8" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B77" s="1" t="s">
+    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B78" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="C77" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E77" s="8" t="s">
+      <c r="C78" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E78" s="8" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="78" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B78" s="1" t="s">
+    <row r="79" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B79" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="C78" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D78" s="1" t="s">
+      <c r="C79" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D79" s="1" t="s">
         <v>223</v>
-      </c>
-      <c r="E78" s="8" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="79" spans="2:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="B79" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>225</v>
       </c>
       <c r="E79" s="8" t="s">
         <v>226</v>
       </c>
-      <c r="F79" s="2" t="s">
+    </row>
+    <row r="80" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="B80" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="E80" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="F80" s="2" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="80" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B80" s="1" t="s">
+    <row r="81" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B81" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="C80" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D80" s="1" t="s">
+      <c r="C81" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D81" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="E80" s="8" t="s">
+      <c r="E81" s="8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="81" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B81" s="1" t="s">
+    <row r="82" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B82" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="D81" s="1" t="s">
+      <c r="D82" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="E81" s="8" t="s">
+      <c r="E82" s="8" t="s">
         <v>232</v>
-      </c>
-    </row>
-    <row r="82" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B82" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="E82" s="8" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="83" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B83" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="E83" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="84" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B84" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E83" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="F83" s="2" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="84" spans="2:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="B84" s="1" t="s">
-        <v>237</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>238</v>
+        <v>53</v>
       </c>
       <c r="E84" s="8" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="85" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="85" spans="2:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B85" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D85" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="E85" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="86" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B86" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D86" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E85" s="8" t="s">
+      <c r="E86" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="F85" s="2" t="s">
+      <c r="F86" s="2" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="86" spans="2:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="B86" s="1" t="s">
+    <row r="87" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="B87" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="C86" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D86" s="1" t="s">
+      <c r="C87" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D87" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="E86" s="8" t="s">
+      <c r="E87" s="8" t="s">
         <v>246</v>
       </c>
-      <c r="F86" s="2" t="s">
+      <c r="F87" s="2" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="87" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B87" s="1" t="s">
+    <row r="88" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B88" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="C87" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D87" s="1" t="s">
+      <c r="C88" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D88" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="E87" s="8" t="s">
+      <c r="E88" s="8" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="88" spans="2:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="B88" s="1" t="s">
+    <row r="89" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="B89" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="C88" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D88" s="1" t="s">
+      <c r="C89" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D89" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="E88" s="8" t="s">
+      <c r="E89" s="8" t="s">
         <v>252</v>
       </c>
-      <c r="F88" s="2" t="s">
+      <c r="F89" s="2" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="89" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B89" s="1" t="s">
+    <row r="90" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B90" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="C89" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D89" s="1" t="s">
+      <c r="C90" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D90" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="E89" s="8" t="s">
+      <c r="E90" s="8" t="s">
         <v>256</v>
       </c>
-      <c r="F89" s="2" t="s">
+      <c r="F90" s="2" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="90" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B90" s="1" t="s">
+    <row r="91" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B91" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="C90" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D90" s="1" t="s">
+      <c r="C91" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D91" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="E90" s="8" t="s">
+      <c r="E91" s="8" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="91" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B91" s="1" t="s">
+    <row r="92" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B92" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="C91" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D91" s="1" t="s">
+      <c r="C92" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D92" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="E91" s="8" t="s">
+      <c r="E92" s="8" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="92" spans="2:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="B92" s="1" t="s">
+    <row r="93" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="B93" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="C92" s="1" t="s">
+      <c r="C93" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D92" s="1" t="s">
+      <c r="D93" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="E92" s="8" t="s">
+      <c r="E93" s="8" t="s">
         <v>264</v>
       </c>
-      <c r="F92" s="2" t="s">
+      <c r="F93" s="2" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="93" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B93" s="1" t="s">
+    <row r="94" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B94" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="C93" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D93" s="1" t="s">
+      <c r="C94" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D94" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="E93" s="8" t="s">
+      <c r="E94" s="8" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="94" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B94" s="1" t="s">
+    <row r="95" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B95" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="C94" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D94" s="1" t="s">
+      <c r="C95" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D95" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="E94" s="8" t="s">
+      <c r="E95" s="8" t="s">
         <v>271</v>
-      </c>
-    </row>
-    <row r="95" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B95" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D95" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="E95" s="8" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="96" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B96" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="E96" s="8" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="97" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B97" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="C96" s="1" t="s">
+      <c r="C97" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="D96" s="8" t="s">
+      <c r="D97" s="8" t="s">
         <v>277</v>
       </c>
-      <c r="E96" s="1" t="s">
+      <c r="E97" s="1" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="97" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B97" s="1" t="s">
+    <row r="98" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B98" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="C97" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D97" s="1" t="s">
+      <c r="C98" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D98" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="E97" s="8" t="s">
+      <c r="E98" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="F97" s="2" t="s">
+      <c r="F98" s="2" t="s">
         <v>280</v>
-      </c>
-    </row>
-    <row r="98" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B98" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="E98" s="8" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="99" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B99" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="E99" s="8" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="100" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B100" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="C99" s="1" t="s">
+      <c r="C100" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="D99" s="1" t="s">
+      <c r="D100" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="E99" s="8" t="s">
+      <c r="E100" s="8" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="100" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B100" s="1" t="s">
+    <row r="101" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B101" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="C100" s="1" t="s">
+      <c r="C101" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="D100" s="1" t="s">
+      <c r="D101" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="E100" s="8" t="s">
+      <c r="E101" s="8" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="101" spans="2:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="B101" s="1" t="s">
+    <row r="102" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="B102" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="C101" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D101" s="1" t="s">
+      <c r="C102" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D102" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="E101" s="8" t="s">
+      <c r="E102" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="F101" s="2" t="s">
+      <c r="F102" s="2" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="102" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B102" s="1" t="s">
+    <row r="103" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B103" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="C102" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D102" s="1" t="s">
+      <c r="C103" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D103" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="E102" s="8" t="s">
+      <c r="E103" s="8" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="103" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B103" s="1" t="s">
+    <row r="104" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B104" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="C103" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D103" s="1" t="s">
+      <c r="C104" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D104" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="E103" s="8" t="s">
+      <c r="E104" s="8" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="104" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B104" s="1" t="s">
+    <row r="105" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B105" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="C104" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D104" s="1" t="s">
+      <c r="C105" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D105" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="E104" s="8" t="s">
+      <c r="E105" s="8" t="s">
         <v>303</v>
-      </c>
-    </row>
-    <row r="105" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B105" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="C105" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="D105" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="E105" s="8" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="106" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B106" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="E106" s="8" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="107" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B107" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="C106" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D106" s="1" t="s">
+      <c r="C107" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D107" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="E106" s="8" t="s">
+      <c r="E107" s="8" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="107" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B107" s="1" t="s">
+    <row r="108" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B108" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="C107" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D107" s="1" t="s">
+      <c r="C108" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D108" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="E107" s="8" t="s">
+      <c r="E108" s="8" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="108" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B108" s="1" t="s">
+    <row r="109" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B109" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="C108" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D108" s="1" t="s">
+      <c r="C109" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D109" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="E108" s="8" t="s">
+      <c r="E109" s="8" t="s">
         <v>315</v>
       </c>
-      <c r="F108" s="2" t="s">
+      <c r="F109" s="2" t="s">
         <v>314</v>
-      </c>
-    </row>
-    <row r="109" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B109" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="C109" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D109" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="E109" s="8" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="110" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B110" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="E110" s="8" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="111" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B111" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="C110" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D110" s="1" t="s">
+      <c r="C111" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D111" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="E110" s="8" t="s">
+      <c r="E111" s="8" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="111" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B111" s="1" t="s">
+    <row r="112" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B112" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="C111" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D111" s="1" t="s">
+      <c r="C112" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D112" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="E111" s="8" t="s">
+      <c r="E112" s="8" t="s">
         <v>322</v>
-      </c>
-    </row>
-    <row r="112" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B112" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="C112" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="D112" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="E112" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="F112" s="2" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="113" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B113" s="1" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>19</v>
+        <v>324</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="E113" s="8" t="s">
-        <v>329</v>
+        <v>71</v>
+      </c>
+      <c r="F113" s="2" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="114" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B114" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="E114" s="8" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="115" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B115" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="C114" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D114" s="1" t="s">
+      <c r="C115" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D115" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="E114" s="8" t="s">
+      <c r="E115" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="F114" s="2" t="s">
+      <c r="F115" s="2" t="s">
         <v>332</v>
-      </c>
-    </row>
-    <row r="115" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B115" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="C115" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D115" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="E115" s="8" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="116" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B116" s="1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="E116" s="8" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="117" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B117" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="E117" s="8" t="s">
-        <v>41</v>
+        <v>338</v>
       </c>
     </row>
     <row r="118" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B118" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="E118" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="119" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B119" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="C118" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D118" s="1" t="s">
+      <c r="C119" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D119" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="E118" s="8" t="s">
+      <c r="E119" s="8" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="119" spans="2:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="E119" s="10"/>
+    <row r="120" spans="2:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E120" s="10"/>
+    </row>
+    <row r="121" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B121" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C121" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D121" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E121" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F121" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3178,21 +3212,21 @@
     <hyperlink ref="F29" r:id="rId9"/>
     <hyperlink ref="F36" r:id="rId10"/>
     <hyperlink ref="F38" r:id="rId11"/>
-    <hyperlink ref="F65" r:id="rId12"/>
-    <hyperlink ref="F75" r:id="rId13"/>
-    <hyperlink ref="F79" r:id="rId14"/>
-    <hyperlink ref="F83" r:id="rId15"/>
-    <hyperlink ref="F84" r:id="rId16"/>
-    <hyperlink ref="F85" r:id="rId17"/>
-    <hyperlink ref="F86" r:id="rId18"/>
-    <hyperlink ref="F88" r:id="rId19"/>
-    <hyperlink ref="F89" r:id="rId20"/>
-    <hyperlink ref="F92" r:id="rId21"/>
-    <hyperlink ref="F108" r:id="rId22"/>
-    <hyperlink ref="F114" r:id="rId23"/>
-    <hyperlink ref="F112" r:id="rId24"/>
-    <hyperlink ref="F101" r:id="rId25"/>
-    <hyperlink ref="F97" r:id="rId26"/>
+    <hyperlink ref="F66" r:id="rId12"/>
+    <hyperlink ref="F76" r:id="rId13"/>
+    <hyperlink ref="F80" r:id="rId14"/>
+    <hyperlink ref="F84" r:id="rId15"/>
+    <hyperlink ref="F85" r:id="rId16"/>
+    <hyperlink ref="F86" r:id="rId17"/>
+    <hyperlink ref="F87" r:id="rId18"/>
+    <hyperlink ref="F89" r:id="rId19"/>
+    <hyperlink ref="F90" r:id="rId20"/>
+    <hyperlink ref="F93" r:id="rId21"/>
+    <hyperlink ref="F109" r:id="rId22"/>
+    <hyperlink ref="F115" r:id="rId23"/>
+    <hyperlink ref="F113" r:id="rId24"/>
+    <hyperlink ref="F102" r:id="rId25"/>
+    <hyperlink ref="F98" r:id="rId26"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>